<commit_message>
Update to SerialConnection script
</commit_message>
<xml_diff>
--- a/S2T/BASELINE/S2T/product_specific/dmr/LoggerFiles/TileView_Template.xlsx
+++ b/S2T/BASELINE/S2T/product_specific/dmr/LoggerFiles/TileView_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Automation\Automation\S2T\BASELINE\S2T\product_specific\dmr\LoggerFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3045465-8D7F-415F-8DC9-74D3CEB24C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A055D8-DD64-4596-BB21-3228F454D2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3DA75837-8C0C-4B6E-9F29-CC335C1414E1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DA75837-8C0C-4B6E-9F29-CC335C1414E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -1557,11 +1557,98 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1590,95 +1677,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1689,8 +1689,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2187,28 +2187,28 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
@@ -2218,20 +2218,20 @@
     </row>
     <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
       <c r="P3" s="58"/>
       <c r="Q3" s="59"/>
       <c r="R3" s="59"/>
@@ -2247,26 +2247,26 @@
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="67" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70" t="s">
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="72"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="49"/>
       <c r="P4" s="60"/>
       <c r="Q4" s="60"/>
       <c r="R4" s="60"/>
@@ -2282,10 +2282,10 @@
     </row>
     <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
-      <c r="B5" s="47">
+      <c r="B5" s="51">
         <v>0</v>
       </c>
-      <c r="C5" s="48"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="23" t="s">
         <v>15</v>
       </c>
@@ -2337,10 +2337,10 @@
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="44">
         <v>0</v>
       </c>
       <c r="D6" s="23">
@@ -2394,8 +2394,8 @@
     </row>
     <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="23">
         <v>1</v>
       </c>
@@ -2447,8 +2447,8 @@
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="35">
+      <c r="B8" s="36"/>
+      <c r="C8" s="44">
         <v>1</v>
       </c>
       <c r="D8" s="23">
@@ -2502,8 +2502,8 @@
     </row>
     <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="50"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="23">
         <v>3</v>
       </c>
@@ -2555,8 +2555,8 @@
     </row>
     <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="35">
+      <c r="B10" s="36"/>
+      <c r="C10" s="44">
         <v>2</v>
       </c>
       <c r="D10" s="23">
@@ -2610,8 +2610,8 @@
     </row>
     <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="23">
         <v>5</v>
       </c>
@@ -2663,8 +2663,8 @@
     </row>
     <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="35">
+      <c r="B12" s="36"/>
+      <c r="C12" s="44">
         <v>3</v>
       </c>
       <c r="D12" s="23">
@@ -2718,8 +2718,8 @@
     </row>
     <row r="13" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -2771,21 +2771,21 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="74"/>
       <c r="J14" s="30"/>
-      <c r="K14" s="52" t="s">
+      <c r="K14" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="54"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="40"/>
       <c r="O14" s="31"/>
       <c r="P14" s="60"/>
       <c r="Q14" s="60"/>
@@ -2802,14 +2802,14 @@
     </row>
     <row r="15" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
-      <c r="B15" s="73"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="42"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="71"/>
       <c r="J15" s="32"/>
       <c r="K15" s="33" t="s">
         <v>19</v>
@@ -2839,20 +2839,20 @@
     </row>
     <row r="16" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="66"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
       <c r="P16" s="61"/>
       <c r="Q16" s="60"/>
       <c r="R16" s="60"/>
@@ -2868,26 +2868,26 @@
     </row>
     <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="67" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="70" t="s">
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="72"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="49"/>
       <c r="P17" s="60"/>
       <c r="Q17" s="60"/>
       <c r="R17" s="60"/>
@@ -2903,10 +2903,10 @@
     </row>
     <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
-      <c r="B18" s="47">
+      <c r="B18" s="51">
         <v>1</v>
       </c>
-      <c r="C18" s="49"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="23" t="s">
         <v>15</v>
       </c>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="19" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="44">
         <v>0</v>
       </c>
       <c r="D19" s="23">
@@ -3015,8 +3015,8 @@
     </row>
     <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="50"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="23">
         <v>1</v>
       </c>
@@ -3068,8 +3068,8 @@
     </row>
     <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="35">
+      <c r="B21" s="36"/>
+      <c r="C21" s="44">
         <v>1</v>
       </c>
       <c r="D21" s="23">
@@ -3123,8 +3123,8 @@
     </row>
     <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="50"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="23">
         <v>3</v>
       </c>
@@ -3176,8 +3176,8 @@
     </row>
     <row r="23" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="35">
+      <c r="B23" s="36"/>
+      <c r="C23" s="44">
         <v>2</v>
       </c>
       <c r="D23" s="23">
@@ -3231,8 +3231,8 @@
     </row>
     <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="50"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="23">
         <v>5</v>
       </c>
@@ -3284,8 +3284,8 @@
     </row>
     <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="35">
+      <c r="B25" s="36"/>
+      <c r="C25" s="44">
         <v>3</v>
       </c>
       <c r="D25" s="23">
@@ -3339,8 +3339,8 @@
     </row>
     <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="46"/>
       <c r="D26" s="24">
         <v>7</v>
       </c>
@@ -3392,21 +3392,21 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
-      <c r="B27" s="63"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="39"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="68"/>
       <c r="J27" s="30"/>
-      <c r="K27" s="52" t="s">
+      <c r="K27" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="54"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="40"/>
       <c r="O27" s="31"/>
       <c r="P27" s="60"/>
       <c r="Q27" s="60"/>
@@ -3423,14 +3423,14 @@
     </row>
     <row r="28" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
-      <c r="B28" s="73"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="14"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="42"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71"/>
       <c r="J28" s="32"/>
       <c r="K28" s="33" t="s">
         <v>19</v>
@@ -3460,20 +3460,20 @@
     </row>
     <row r="29" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="66"/>
-      <c r="L29" s="66"/>
-      <c r="M29" s="66"/>
-      <c r="N29" s="66"/>
-      <c r="O29" s="66"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
       <c r="P29" s="61"/>
       <c r="Q29" s="60"/>
       <c r="R29" s="60"/>
@@ -3489,26 +3489,26 @@
     </row>
     <row r="30" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="67" t="s">
+      <c r="C30" s="52"/>
+      <c r="D30" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="70" t="s">
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="71"/>
-      <c r="L30" s="71"/>
-      <c r="M30" s="71"/>
-      <c r="N30" s="71"/>
-      <c r="O30" s="72"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="49"/>
       <c r="P30" s="60"/>
       <c r="Q30" s="60"/>
       <c r="R30" s="60"/>
@@ -3524,10 +3524,10 @@
     </row>
     <row r="31" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
-      <c r="B31" s="47">
+      <c r="B31" s="51">
         <v>2</v>
       </c>
-      <c r="C31" s="49"/>
+      <c r="C31" s="53"/>
       <c r="D31" s="23" t="s">
         <v>15</v>
       </c>
@@ -3579,10 +3579,10 @@
     </row>
     <row r="32" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="35">
+      <c r="C32" s="44">
         <v>0</v>
       </c>
       <c r="D32" s="23">
@@ -3636,8 +3636,8 @@
     </row>
     <row r="33" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="50"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="23">
         <v>1</v>
       </c>
@@ -3689,8 +3689,8 @@
     </row>
     <row r="34" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="35">
+      <c r="B34" s="36"/>
+      <c r="C34" s="44">
         <v>1</v>
       </c>
       <c r="D34" s="23">
@@ -3744,8 +3744,8 @@
     </row>
     <row r="35" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="50"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="23">
         <v>3</v>
       </c>
@@ -3797,8 +3797,8 @@
     </row>
     <row r="36" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="35">
+      <c r="B36" s="36"/>
+      <c r="C36" s="44">
         <v>2</v>
       </c>
       <c r="D36" s="23">
@@ -3852,8 +3852,8 @@
     </row>
     <row r="37" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="50"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="23">
         <v>5</v>
       </c>
@@ -3905,8 +3905,8 @@
     </row>
     <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="35">
+      <c r="B38" s="36"/>
+      <c r="C38" s="44">
         <v>3</v>
       </c>
       <c r="D38" s="23">
@@ -3960,8 +3960,8 @@
     </row>
     <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="46"/>
       <c r="D39" s="24">
         <v>7</v>
       </c>
@@ -4013,21 +4013,21 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
-      <c r="B40" s="63"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="68"/>
       <c r="J40" s="30"/>
-      <c r="K40" s="52" t="s">
+      <c r="K40" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="54"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="40"/>
       <c r="O40" s="31"/>
       <c r="P40" s="60"/>
       <c r="Q40" s="60"/>
@@ -4044,14 +4044,14 @@
     </row>
     <row r="41" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11"/>
-      <c r="B41" s="73"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="14"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="42"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="71"/>
       <c r="J41" s="32"/>
       <c r="K41" s="33" t="s">
         <v>19</v>
@@ -4081,20 +4081,20 @@
     </row>
     <row r="42" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="66"/>
-      <c r="O42" s="66"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="43"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
       <c r="P42" s="61"/>
       <c r="Q42" s="60"/>
       <c r="R42" s="60"/>
@@ -4110,26 +4110,26 @@
     </row>
     <row r="43" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11"/>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="67" t="s">
+      <c r="C43" s="52"/>
+      <c r="D43" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="70" t="s">
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K43" s="71"/>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="71"/>
-      <c r="O43" s="72"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="49"/>
       <c r="P43" s="60"/>
       <c r="Q43" s="60"/>
       <c r="R43" s="60"/>
@@ -4145,10 +4145,10 @@
     </row>
     <row r="44" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11"/>
-      <c r="B44" s="47">
+      <c r="B44" s="51">
         <v>3</v>
       </c>
-      <c r="C44" s="49"/>
+      <c r="C44" s="53"/>
       <c r="D44" s="23" t="s">
         <v>15</v>
       </c>
@@ -4200,10 +4200,10 @@
     </row>
     <row r="45" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11"/>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="35">
+      <c r="C45" s="44">
         <v>0</v>
       </c>
       <c r="D45" s="23">
@@ -4257,8 +4257,8 @@
     </row>
     <row r="46" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="50"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="45"/>
       <c r="D46" s="23">
         <v>1</v>
       </c>
@@ -4310,8 +4310,8 @@
     </row>
     <row r="47" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="35">
+      <c r="B47" s="36"/>
+      <c r="C47" s="44">
         <v>1</v>
       </c>
       <c r="D47" s="23">
@@ -4365,8 +4365,8 @@
     </row>
     <row r="48" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="50"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="45"/>
       <c r="D48" s="23">
         <v>3</v>
       </c>
@@ -4418,8 +4418,8 @@
     </row>
     <row r="49" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="35">
+      <c r="B49" s="36"/>
+      <c r="C49" s="44">
         <v>2</v>
       </c>
       <c r="D49" s="23">
@@ -4473,8 +4473,8 @@
     </row>
     <row r="50" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="50"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="45"/>
       <c r="D50" s="23">
         <v>5</v>
       </c>
@@ -4526,8 +4526,8 @@
     </row>
     <row r="51" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="35">
+      <c r="B51" s="36"/>
+      <c r="C51" s="44">
         <v>3</v>
       </c>
       <c r="D51" s="23">
@@ -4581,8 +4581,8 @@
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="36"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="46"/>
       <c r="D52" s="24">
         <v>7</v>
       </c>
@@ -4634,21 +4634,21 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
-      <c r="B53" s="63"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="14"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="39"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="67"/>
+      <c r="I53" s="68"/>
       <c r="J53" s="30"/>
-      <c r="K53" s="52" t="s">
+      <c r="K53" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="L53" s="53"/>
-      <c r="M53" s="53"/>
-      <c r="N53" s="54"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="39"/>
+      <c r="N53" s="40"/>
       <c r="O53" s="31"/>
       <c r="P53" s="60"/>
       <c r="Q53" s="60"/>
@@ -4665,14 +4665,14 @@
     </row>
     <row r="54" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11"/>
-      <c r="B54" s="63"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="14"/>
-      <c r="D54" s="40"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="41"/>
-      <c r="I54" s="42"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="71"/>
       <c r="J54" s="32"/>
       <c r="K54" s="33" t="s">
         <v>19</v>
@@ -5284,20 +5284,20 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" s="11"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
-      <c r="I69" s="65"/>
-      <c r="J69" s="65"/>
-      <c r="K69" s="65"/>
-      <c r="L69" s="65"/>
-      <c r="M69" s="65"/>
-      <c r="N69" s="65"/>
-      <c r="O69" s="65"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="42"/>
+      <c r="J69" s="42"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="42"/>
+      <c r="O69" s="42"/>
       <c r="P69" s="61"/>
       <c r="Q69" s="60"/>
       <c r="R69" s="60"/>
@@ -5313,26 +5313,26 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
-      <c r="B70" s="74"/>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="74"/>
-      <c r="K70" s="74"/>
-      <c r="L70" s="74"/>
-      <c r="M70" s="74"/>
-      <c r="N70" s="74"/>
-      <c r="O70" s="74"/>
-      <c r="P70" s="74"/>
-      <c r="Q70" s="74"/>
-      <c r="R70" s="74"/>
-      <c r="S70" s="74"/>
-      <c r="T70" s="74"/>
-      <c r="U70" s="74"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="50"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="50"/>
+      <c r="M70" s="50"/>
+      <c r="N70" s="50"/>
+      <c r="O70" s="50"/>
+      <c r="P70" s="50"/>
+      <c r="Q70" s="50"/>
+      <c r="R70" s="50"/>
+      <c r="S70" s="50"/>
+      <c r="T70" s="50"/>
+      <c r="U70" s="50"/>
       <c r="V70" s="11"/>
       <c r="W70" s="11"/>
       <c r="X70" s="11"/>
@@ -5989,28 +5989,22 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="B29:O29"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="B32:B41"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="B70:U70"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D53:I54"/>
+    <mergeCell ref="D40:I41"/>
+    <mergeCell ref="D27:I28"/>
+    <mergeCell ref="D14:I15"/>
+    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="J17:O17"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="K53:N53"/>
     <mergeCell ref="B62:O62"/>
@@ -6027,23 +6021,29 @@
     <mergeCell ref="D4:I4"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="B32:B41"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="B70:U70"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
     <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D53:I54"/>
-    <mergeCell ref="D40:I41"/>
-    <mergeCell ref="D27:I28"/>
-    <mergeCell ref="D14:I15"/>
-    <mergeCell ref="D30:I30"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E6:I13 K14 E19:I26 K19:N26 E32:I39 K32:N39">
@@ -6145,28 +6145,28 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
       <c r="X2" s="11"/>
@@ -6176,20 +6176,20 @@
     </row>
     <row r="3" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
       <c r="P3" s="58"/>
       <c r="Q3" s="59"/>
       <c r="R3" s="59"/>
@@ -6205,26 +6205,26 @@
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="68" t="s">
+      <c r="C4" s="52"/>
+      <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="70" t="s">
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="79"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="75"/>
       <c r="P4" s="61"/>
       <c r="Q4" s="60"/>
       <c r="R4" s="60"/>
@@ -6240,10 +6240,10 @@
     </row>
     <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
-      <c r="B5" s="47">
+      <c r="B5" s="51">
         <v>0</v>
       </c>
-      <c r="C5" s="75"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
@@ -6295,10 +6295,10 @@
     </row>
     <row r="6" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="62">
+      <c r="C6" s="35">
         <v>0</v>
       </c>
       <c r="D6" s="23">
@@ -6360,8 +6360,8 @@
     </row>
     <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="23">
         <v>1</v>
       </c>
@@ -6421,8 +6421,8 @@
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="62">
+      <c r="B8" s="36"/>
+      <c r="C8" s="35">
         <v>1</v>
       </c>
       <c r="D8" s="23">
@@ -6484,8 +6484,8 @@
     </row>
     <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="23">
         <v>3</v>
       </c>
@@ -6545,8 +6545,8 @@
     </row>
     <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="62">
+      <c r="B10" s="36"/>
+      <c r="C10" s="35">
         <v>2</v>
       </c>
       <c r="D10" s="23">
@@ -6608,8 +6608,8 @@
     </row>
     <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="23">
         <v>5</v>
       </c>
@@ -6669,8 +6669,8 @@
     </row>
     <row r="12" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="62">
+      <c r="B12" s="36"/>
+      <c r="C12" s="35">
         <v>3</v>
       </c>
       <c r="D12" s="23">
@@ -6732,8 +6732,8 @@
     </row>
     <row r="13" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="24">
         <v>7</v>
       </c>
@@ -6793,7 +6793,7 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
-      <c r="B14" s="63"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="14"/>
       <c r="D14" s="6"/>
       <c r="E14" s="22"/>
@@ -6824,7 +6824,7 @@
     </row>
     <row r="15" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
-      <c r="B15" s="73"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="14"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
@@ -6861,20 +6861,20 @@
     </row>
     <row r="16" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="65"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
       <c r="P16" s="61"/>
       <c r="Q16" s="60"/>
       <c r="R16" s="60"/>
@@ -6890,26 +6890,26 @@
     </row>
     <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="68" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="70" t="s">
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="79"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="75"/>
       <c r="P17" s="61"/>
       <c r="Q17" s="60"/>
       <c r="R17" s="60"/>
@@ -6925,10 +6925,10 @@
     </row>
     <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
-      <c r="B18" s="47">
+      <c r="B18" s="51">
         <v>1</v>
       </c>
-      <c r="C18" s="75"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="23" t="s">
         <v>15</v>
       </c>
@@ -6980,10 +6980,10 @@
     </row>
     <row r="19" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11"/>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="62">
+      <c r="C19" s="35">
         <v>0</v>
       </c>
       <c r="D19" s="23">
@@ -7045,8 +7045,8 @@
     </row>
     <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="23">
         <v>1</v>
       </c>
@@ -7106,8 +7106,8 @@
     </row>
     <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="62">
+      <c r="B21" s="36"/>
+      <c r="C21" s="35">
         <v>1</v>
       </c>
       <c r="D21" s="23">
@@ -7169,8 +7169,8 @@
     </row>
     <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="23">
         <v>3</v>
       </c>
@@ -7230,8 +7230,8 @@
     </row>
     <row r="23" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="62">
+      <c r="B23" s="36"/>
+      <c r="C23" s="35">
         <v>2</v>
       </c>
       <c r="D23" s="23">
@@ -7293,8 +7293,8 @@
     </row>
     <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="23">
         <v>5</v>
       </c>
@@ -7354,8 +7354,8 @@
     </row>
     <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="62">
+      <c r="B25" s="36"/>
+      <c r="C25" s="35">
         <v>3</v>
       </c>
       <c r="D25" s="23">
@@ -7417,8 +7417,8 @@
     </row>
     <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="24">
         <v>7</v>
       </c>
@@ -7478,7 +7478,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
-      <c r="B27" s="63"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="14"/>
       <c r="D27" s="6"/>
       <c r="E27" s="22"/>
@@ -7509,7 +7509,7 @@
     </row>
     <row r="28" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
-      <c r="B28" s="73"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="14"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
@@ -7546,20 +7546,20 @@
     </row>
     <row r="29" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="65"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="65"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
       <c r="P29" s="61"/>
       <c r="Q29" s="60"/>
       <c r="R29" s="60"/>
@@ -7575,26 +7575,26 @@
     </row>
     <row r="30" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="68" t="s">
+      <c r="C30" s="52"/>
+      <c r="D30" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="70" t="s">
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="71"/>
-      <c r="L30" s="71"/>
-      <c r="M30" s="71"/>
-      <c r="N30" s="71"/>
-      <c r="O30" s="79"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="75"/>
       <c r="P30" s="61"/>
       <c r="Q30" s="60"/>
       <c r="R30" s="60"/>
@@ -7610,10 +7610,10 @@
     </row>
     <row r="31" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
-      <c r="B31" s="47">
+      <c r="B31" s="51">
         <v>2</v>
       </c>
-      <c r="C31" s="75"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="23" t="s">
         <v>15</v>
       </c>
@@ -7665,10 +7665,10 @@
     </row>
     <row r="32" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="62">
+      <c r="C32" s="35">
         <v>0</v>
       </c>
       <c r="D32" s="23">
@@ -7730,8 +7730,8 @@
     </row>
     <row r="33" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="23">
         <v>1</v>
       </c>
@@ -7791,8 +7791,8 @@
     </row>
     <row r="34" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="62">
+      <c r="B34" s="36"/>
+      <c r="C34" s="35">
         <v>1</v>
       </c>
       <c r="D34" s="23">
@@ -7854,8 +7854,8 @@
     </row>
     <row r="35" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
       <c r="D35" s="23">
         <v>3</v>
       </c>
@@ -7915,8 +7915,8 @@
     </row>
     <row r="36" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="62">
+      <c r="B36" s="36"/>
+      <c r="C36" s="35">
         <v>2</v>
       </c>
       <c r="D36" s="23">
@@ -7978,8 +7978,8 @@
     </row>
     <row r="37" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="23">
         <v>5</v>
       </c>
@@ -8039,8 +8039,8 @@
     </row>
     <row r="38" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="62">
+      <c r="B38" s="36"/>
+      <c r="C38" s="35">
         <v>3</v>
       </c>
       <c r="D38" s="23">
@@ -8102,8 +8102,8 @@
     </row>
     <row r="39" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
       <c r="D39" s="24">
         <v>7</v>
       </c>
@@ -8163,7 +8163,7 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
-      <c r="B40" s="63"/>
+      <c r="B40" s="36"/>
       <c r="C40" s="14"/>
       <c r="D40" s="6"/>
       <c r="E40" s="22"/>
@@ -8194,7 +8194,7 @@
     </row>
     <row r="41" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11"/>
-      <c r="B41" s="73"/>
+      <c r="B41" s="37"/>
       <c r="C41" s="14"/>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
@@ -8231,20 +8231,20 @@
     </row>
     <row r="42" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="65"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="65"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
       <c r="P42" s="61"/>
       <c r="Q42" s="60"/>
       <c r="R42" s="60"/>
@@ -8260,26 +8260,26 @@
     </row>
     <row r="43" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11"/>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="68" t="s">
+      <c r="C43" s="52"/>
+      <c r="D43" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="70" t="s">
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="K43" s="71"/>
-      <c r="L43" s="71"/>
-      <c r="M43" s="71"/>
-      <c r="N43" s="71"/>
-      <c r="O43" s="79"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="75"/>
       <c r="P43" s="61"/>
       <c r="Q43" s="60"/>
       <c r="R43" s="60"/>
@@ -8295,10 +8295,10 @@
     </row>
     <row r="44" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11"/>
-      <c r="B44" s="47">
+      <c r="B44" s="51">
         <v>3</v>
       </c>
-      <c r="C44" s="75"/>
+      <c r="C44" s="79"/>
       <c r="D44" s="23" t="s">
         <v>15</v>
       </c>
@@ -8350,10 +8350,10 @@
     </row>
     <row r="45" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11"/>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="62">
+      <c r="C45" s="35">
         <v>0</v>
       </c>
       <c r="D45" s="23">
@@ -8415,8 +8415,8 @@
     </row>
     <row r="46" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
       <c r="D46" s="23">
         <v>1</v>
       </c>
@@ -8476,8 +8476,8 @@
     </row>
     <row r="47" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="62">
+      <c r="B47" s="36"/>
+      <c r="C47" s="35">
         <v>1</v>
       </c>
       <c r="D47" s="23">
@@ -8539,8 +8539,8 @@
     </row>
     <row r="48" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="63"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="23">
         <v>3</v>
       </c>
@@ -8600,8 +8600,8 @@
     </row>
     <row r="49" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="62">
+      <c r="B49" s="36"/>
+      <c r="C49" s="35">
         <v>2</v>
       </c>
       <c r="D49" s="23">
@@ -8663,8 +8663,8 @@
     </row>
     <row r="50" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="63"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
       <c r="D50" s="23">
         <v>5</v>
       </c>
@@ -8724,8 +8724,8 @@
     </row>
     <row r="51" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="62">
+      <c r="B51" s="36"/>
+      <c r="C51" s="35">
         <v>3</v>
       </c>
       <c r="D51" s="23">
@@ -8787,8 +8787,8 @@
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
       <c r="D52" s="24">
         <v>7</v>
       </c>
@@ -8848,7 +8848,7 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
-      <c r="B53" s="63"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="14"/>
       <c r="D53" s="6"/>
       <c r="E53" s="22"/>
@@ -8879,7 +8879,7 @@
     </row>
     <row r="54" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11"/>
-      <c r="B54" s="63"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="14"/>
       <c r="D54" s="19"/>
       <c r="E54" s="20"/>
@@ -9498,20 +9498,20 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" s="11"/>
-      <c r="B69" s="64"/>
-      <c r="C69" s="64"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
-      <c r="I69" s="65"/>
-      <c r="J69" s="65"/>
-      <c r="K69" s="65"/>
-      <c r="L69" s="65"/>
-      <c r="M69" s="65"/>
-      <c r="N69" s="65"/>
-      <c r="O69" s="65"/>
+      <c r="B69" s="41"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="42"/>
+      <c r="J69" s="42"/>
+      <c r="K69" s="42"/>
+      <c r="L69" s="42"/>
+      <c r="M69" s="42"/>
+      <c r="N69" s="42"/>
+      <c r="O69" s="42"/>
       <c r="P69" s="61"/>
       <c r="Q69" s="60"/>
       <c r="R69" s="60"/>
@@ -9527,26 +9527,26 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
-      <c r="B70" s="74"/>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="74"/>
-      <c r="K70" s="74"/>
-      <c r="L70" s="74"/>
-      <c r="M70" s="74"/>
-      <c r="N70" s="74"/>
-      <c r="O70" s="74"/>
-      <c r="P70" s="74"/>
-      <c r="Q70" s="74"/>
-      <c r="R70" s="74"/>
-      <c r="S70" s="74"/>
-      <c r="T70" s="74"/>
-      <c r="U70" s="74"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="50"/>
+      <c r="K70" s="50"/>
+      <c r="L70" s="50"/>
+      <c r="M70" s="50"/>
+      <c r="N70" s="50"/>
+      <c r="O70" s="50"/>
+      <c r="P70" s="50"/>
+      <c r="Q70" s="50"/>
+      <c r="R70" s="50"/>
+      <c r="S70" s="50"/>
+      <c r="T70" s="50"/>
+      <c r="U70" s="50"/>
       <c r="V70" s="11"/>
       <c r="W70" s="11"/>
       <c r="X70" s="11"/>
@@ -10203,20 +10203,17 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="J43:O43"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="B29:O29"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B42:O42"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B69:O69"/>
+    <mergeCell ref="B70:U70"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="B55:O55"/>
+    <mergeCell ref="B62:O62"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="B3:O3"/>
@@ -10233,6 +10230,15 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:I17"/>
     <mergeCell ref="J17:O17"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B42:O42"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:I30"/>
     <mergeCell ref="J30:O30"/>
@@ -10240,20 +10246,14 @@
     <mergeCell ref="B32:B41"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="J43:O43"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="B29:O29"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="K40:N40"/>
-    <mergeCell ref="B69:O69"/>
-    <mergeCell ref="B70:U70"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:B54"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="B55:O55"/>
-    <mergeCell ref="B62:O62"/>
   </mergeCells>
   <conditionalFormatting sqref="E6:I14 K14 K19:N26 E19:I27 K32:N39 E32:I40">
     <cfRule type="expression" dxfId="8" priority="7">

</xml_diff>